<commit_message>
updated and integrated workflows
</commit_message>
<xml_diff>
--- a/Project 3/Template.xlsx
+++ b/Project 3/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P3_C_Reed\Full Project\Project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\P3\Indeed\Project 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0205863-3570-493A-B1A0-2DBD572F8693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB7F25F-D631-4DB4-96D5-8422B19FEDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2475" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24960" yWindow="1008" windowWidth="17148" windowHeight="11352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>JobTitle</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Number_Of_Job_Search</t>
-  </si>
-  <si>
-    <t>Developer</t>
   </si>
 </sst>
 </file>
@@ -365,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,14 +393,6 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>